<commit_message>
WORK UPDATE ON 13/08/2020#3
</commit_message>
<xml_diff>
--- a/HelpDocuments/Birla New Reports/dedn_template.xlsx
+++ b/HelpDocuments/Birla New Reports/dedn_template.xlsx
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1689,6 +1689,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="E52:H52"/>
     <mergeCell ref="M52:N52"/>
@@ -1698,12 +1704,6 @@
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="E42:H42"/>
     <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>